<commit_message>
Report - Appendix 3
</commit_message>
<xml_diff>
--- a/working_documents/Milestone2/1.Content Inventory.xlsx
+++ b/working_documents/Milestone2/1.Content Inventory.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kris/Dropbox/codefair/working_documents/Milestone2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Content Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -256,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,6 +296,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -733,13 +744,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
@@ -749,7 +763,7 @@
     <col min="6" max="6" width="65.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -769,7 +783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>0</v>
       </c>
@@ -785,7 +799,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>1</v>
       </c>
@@ -803,7 +817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>1.1000000000000001</v>
       </c>
@@ -819,7 +833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>1.2</v>
       </c>
@@ -833,7 +847,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>2</v>
       </c>
@@ -851,7 +865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2.1</v>
       </c>
@@ -867,7 +881,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2.2000000000000002</v>
       </c>
@@ -883,7 +897,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2.2999999999999998</v>
       </c>
@@ -899,7 +913,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2.4</v>
       </c>
@@ -915,7 +929,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>2.5</v>
       </c>
@@ -933,7 +947,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>2.6</v>
       </c>
@@ -951,7 +965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>3</v>
       </c>
@@ -969,7 +983,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>4</v>
       </c>
@@ -985,7 +999,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
         <v>5</v>
       </c>
@@ -1003,7 +1017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>6</v>
       </c>
@@ -1019,7 +1033,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>6.1</v>
       </c>
@@ -1037,7 +1051,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>6.2</v>
       </c>
@@ -1055,7 +1069,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
         <v>7</v>
       </c>
@@ -1071,7 +1085,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>7.1</v>
       </c>
@@ -1085,7 +1099,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>7.2</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
         <v>8</v>
       </c>
@@ -1121,7 +1135,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
         <v>9</v>
       </c>
@@ -1139,7 +1153,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
         <v>10</v>
       </c>
@@ -1157,7 +1171,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
         <v>11</v>
       </c>
@@ -1173,7 +1187,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="4"/>
@@ -1182,11 +1196,8 @@
       <c r="F27" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>